<commit_message>
modify the query time of IS-Label on Lubm2U
</commit_message>
<xml_diff>
--- a/total-query-time.xlsx
+++ b/total-query-time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyb\Desktop\DO4KG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5596775F-7D1A-47D1-B36C-A4507DA977F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9BFF47-8612-4E08-85D4-A29F5B11323D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lubm50U" sheetId="1" r:id="rId1"/>
@@ -1382,8 +1382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4BD135-E580-4AFC-BCD4-322B0E12F533}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -1413,22 +1413,22 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>0.99454399999999998</v>
+        <v>198.491738</v>
       </c>
       <c r="C2" s="1">
-        <v>0.99860300000000002</v>
+        <v>209.02425299999999</v>
       </c>
       <c r="D2" s="1">
-        <v>0.98651</v>
+        <v>198.53247300000001</v>
       </c>
       <c r="E2" s="1">
-        <v>0.98184000000000005</v>
+        <v>197.81455600000001</v>
       </c>
       <c r="F2" s="1">
-        <v>0.96904699999999999</v>
+        <v>197.05119400000001</v>
       </c>
       <c r="G2" s="1">
-        <v>0.98245300000000002</v>
+        <v>198.380337</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1940,7 +1940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51B1A0-B870-4D5B-89B7-8BD2167E9973}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>